<commit_message>
started revision of paper
</commit_message>
<xml_diff>
--- a/Rupture_Data.xlsx
+++ b/Rupture_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_RESEARCH\08_Dynamic Mechanical Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BB1CB0-C6B9-40BB-B100-E76109C56710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E84EF8B-EC2D-434B-9881-D6EF783AF9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="1155" windowWidth="28800" windowHeight="11385" xr2:uid="{2C2E5B4E-3800-44E9-9A42-4B5A272C9F90}"/>
   </bookViews>
@@ -238,17 +238,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,7 +567,7 @@
   <dimension ref="A2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -583,67 +583,67 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="3"/>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14" ht="60">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>